<commit_message>
desde work 01 Sep
</commit_message>
<xml_diff>
--- a/src/assets/rep_marcaciones.xlsx
+++ b/src/assets/rep_marcaciones.xlsx
@@ -20,29 +20,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t xml:space="preserve">    REPORTE DE ASISTENCIA</t>
   </si>
   <si>
-    <t xml:space="preserve">Terminal :</t>
-  </si>
-  <si>
     <t xml:space="preserve">Funcionario:</t>
   </si>
   <si>
-    <t xml:space="preserve">Desde lunes 21 de junio de 2028</t>
+    <t xml:space="preserve">Desde domingo 21 de junio de 2028</t>
   </si>
   <si>
     <t xml:space="preserve">CI:</t>
   </si>
   <si>
-    <t xml:space="preserve">Hasta lunes 20 de julio de 2028</t>
+    <t xml:space="preserve">Hasta domingo 20 de julio de 2028</t>
   </si>
   <si>
     <t xml:space="preserve">Primer Turno</t>
   </si>
   <si>
+    <t xml:space="preserve">SegundoTurno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Retraso</t>
   </si>
   <si>
@@ -64,10 +64,10 @@
     <t xml:space="preserve">[min]</t>
   </si>
   <si>
-    <t xml:space="preserve">Sin Marcar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salió Antes</t>
+    <t xml:space="preserve">SinMarcar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SalióAntes</t>
   </si>
 </sst>
 </file>
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -126,7 +126,7 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -136,6 +136,13 @@
       <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="0"/>
       <charset val="134"/>
     </font>
@@ -224,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -238,18 +245,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -281,31 +276,31 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -334,15 +329,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>332640</xdr:colOff>
+      <xdr:colOff>512640</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1229760</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:colOff>1158120</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -355,8 +350,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="332640" y="0"/>
-          <a:ext cx="897120" cy="847080"/>
+          <a:off x="512640" y="0"/>
+          <a:ext cx="645480" cy="609480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -548,22 +543,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="8.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="6.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.96"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="8.44"/>
   </cols>
   <sheetData>
@@ -587,114 +581,105 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="G3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="G3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="9" t="s">
-        <v>4</v>
-      </c>
+    <row r="4" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="G4" s="8" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="12"/>
+      <c r="G5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="15"/>
-      <c r="B6" s="15"/>
+      <c r="A6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="C6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="16"/>
+        <v>11</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>12</v>
+      </c>
       <c r="E6" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="18"/>
+        <v>11</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="7" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>15</v>
-      </c>
+    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="K7" s="19"/>
     </row>
-    <row r="8" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="14"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="K8" s="22"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="C2:E2"/>
+    <mergeCell ref="G2:I2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="G3:I3"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="H5:I5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="0.590277777777778" bottom="0.590277777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
desde work 02 Sep
</commit_message>
<xml_diff>
--- a/src/assets/rep_marcaciones.xlsx
+++ b/src/assets/rep_marcaciones.xlsx
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -168,12 +168,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -231,7 +225,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,18 +292,6 @@
     </xf>
     <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -335,9 +317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1158120</xdr:colOff>
+      <xdr:colOff>1155960</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:rowOff>47880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -351,7 +333,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="512640" y="0"/>
-          <a:ext cx="645480" cy="609480"/>
+          <a:ext cx="643320" cy="607320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -543,10 +525,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -561,7 +543,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="8.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -587,7 +569,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
         <v>3</v>
       </c>
@@ -609,7 +591,7 @@
       <c r="H4" s="11"/>
       <c r="I4" s="9"/>
     </row>
-    <row r="5" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
@@ -628,7 +610,7 @@
       </c>
       <c r="I5" s="15"/>
     </row>
-    <row r="6" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -657,18 +639,10 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="K7" s="19"/>
-    </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
desde work 03 Sep
</commit_message>
<xml_diff>
--- a/src/assets/rep_marcaciones.xlsx
+++ b/src/assets/rep_marcaciones.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">    REPORTE DE ASISTENCIA</t>
   </si>
@@ -28,13 +28,7 @@
     <t xml:space="preserve">Funcionario:</t>
   </si>
   <si>
-    <t xml:space="preserve">Desde domingo 21 de junio de 2028</t>
-  </si>
-  <si>
     <t xml:space="preserve">CI:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hasta domingo 20 de julio de 2028</t>
   </si>
   <si>
     <t xml:space="preserve">Primer Turno</t>
@@ -317,9 +311,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1155960</xdr:colOff>
+      <xdr:colOff>1154520</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>47880</xdr:rowOff>
+      <xdr:rowOff>46440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -333,7 +327,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="512640" y="0"/>
-          <a:ext cx="643320" cy="607320"/>
+          <a:ext cx="641880" cy="605880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -528,18 +522,16 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="1" width="6.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="6.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="7.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="6.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="8.21"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="8.44"/>
   </cols>
   <sheetData>
@@ -563,22 +555,19 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="G2" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
-      <c r="G3" s="5" t="s">
-        <v>4</v>
-      </c>
+      <c r="G3" s="5"/>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
@@ -595,48 +584,48 @@
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" s="13"/>
       <c r="E5" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F5" s="13"/>
       <c r="G5" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I5" s="15"/>
     </row>
     <row r="6" customFormat="false" ht="14.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="D6" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="E6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="H6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>13</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -647,7 +636,7 @@
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A1:I1"/>
-    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="G3:I3"/>

</xml_diff>